<commit_message>
puse los usuarios y contraseñas correctas
</commit_message>
<xml_diff>
--- a/PAGINA_WEB/usuarios.xlsx
+++ b/PAGINA_WEB/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6C136F-85BF-429A-9AE4-AF7844B2E9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BF77AA-018D-4517-8E94-86F16DF9B722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,27 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Usuario</t>
   </si>
   <si>
     <t>Hash Contraseña (SHA-256)</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>bee103639f6af19b5114f39a0ba4a8631a5ef781697a6b3cc78239cdcfcb8a0e</t>
-  </si>
-  <si>
-    <t>Cin360!!</t>
-  </si>
-  <si>
-    <t>bb98518a655b027ffded743db7901512dc678b47c251aea60c3f37cb783708fc</t>
-  </si>
-  <si>
-    <t>Juli285#!</t>
   </si>
   <si>
     <t>josefina_fernandez</t>
@@ -58,6 +43,18 @@
   </si>
   <si>
     <t>cynthia_lucero</t>
+  </si>
+  <si>
+    <t>62E6BEA9285CD5040EBEB8349FD37884C58FC489083B67AB58F29B142726502B</t>
+  </si>
+  <si>
+    <t>72FB1E6F1436D5A08558E9797A2B048E48468CF7596214E35C8175FD07528F4F</t>
+  </si>
+  <si>
+    <t>D749DD4F4D1390494C0DA15BB5BD1CEE811DA43D6C9D45EA30AA89D95EACC5A5</t>
+  </si>
+  <si>
+    <t>CDF5A0B901FD777EB7A4798AD0872C67546942FA2FEDDD70DE85508162943F31</t>
   </si>
 </sst>
 </file>
@@ -92,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,29 +112,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -359,13 +342,13 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="8.7109375" customWidth="1"/>
@@ -378,42 +361,42 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>